<commit_message>
test: updated tc0011, now also covers applyKcatConstraints and selectKCats
</commit_message>
<xml_diff>
--- a/test/VerificationMatrix.xlsx
+++ b/test/VerificationMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Components\GECKO\Gecko3\GECKO\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A86224-BE9A-44D9-AD30-85A09B9CAC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C216C60D-842B-4E28-BA1C-788B7B384667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
   <si>
     <t>Verification</t>
   </si>
@@ -245,6 +244,15 @@
   </si>
   <si>
     <t>tc0010</t>
+  </si>
+  <si>
+    <t>tc0011</t>
+  </si>
+  <si>
+    <t>partly by tc0011</t>
+  </si>
+  <si>
+    <t>tc0011 - we did not test all possible parameterizations here</t>
   </si>
 </sst>
 </file>
@@ -574,7 +582,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,6 +619,9 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -653,6 +664,9 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -668,10 +682,16 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
test: Added test case for findMetSmiles.
</commit_message>
<xml_diff>
--- a/test/VerificationMatrix.xlsx
+++ b/test/VerificationMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Components\GECKO\Gecko3\GECKO\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C216C60D-842B-4E28-BA1C-788B7B384667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A9ECCC-DF79-4D69-BD35-6FDDA343F975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>Verification</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>tc0011 - we did not test all possible parameterizations here</t>
+  </si>
+  <si>
+    <t>tc0012</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,6 +630,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
test: updated verification matrix
</commit_message>
<xml_diff>
--- a/test/VerificationMatrix.xlsx
+++ b/test/VerificationMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Components\GECKO\Gecko3\GECKO\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D47F99-A67B-47F2-B07B-9CFB56DA813D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD880CA-AEB9-4026-81FC-A0B861C81706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>Verification</t>
   </si>
@@ -250,6 +250,24 @@
   </si>
   <si>
     <t>gather_kcats/getStandardKcat.m</t>
+  </si>
+  <si>
+    <t>tcm0001, tcm0002 - The test doesn't really check the function, only that some output is read</t>
+  </si>
+  <si>
+    <t>tcm0001, tcm0002 - The test doesn't really check the function, only that we get something</t>
+  </si>
+  <si>
+    <t>Has only been tested by running it manually, not tested by test cases</t>
+  </si>
+  <si>
+    <t>tcm0001</t>
+  </si>
+  <si>
+    <t>tcm0001 - does not test all aspects of the adapter, but some.</t>
+  </si>
+  <si>
+    <t>tcm0002 - does not test all aspects of the adapter, but some.</t>
   </si>
 </sst>
 </file>
@@ -578,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,11 +700,17 @@
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -764,6 +788,9 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -785,6 +812,9 @@
       <c r="A27" t="s">
         <v>27</v>
       </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -891,10 +921,16 @@
       <c r="A44" t="s">
         <v>46</v>
       </c>
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>